<commit_message>
test coverage si test link
</commit_message>
<xml_diff>
--- a/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
+++ b/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617BBD23-2529-4AD5-975D-DCDA9F327885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275B1673-C55F-4BF1-9E99-12BA52FCFF80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -1260,7 +1260,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1286,6 +1285,13 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1298,15 +1304,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1334,34 +1346,124 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1400,9 +1502,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1418,106 +1517,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1960,26 +1960,26 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="15" max="15" width="20.19921875" customWidth="1"/>
+    <col min="15" max="15" width="20.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B1" s="12"/>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="41"/>
-    </row>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="B2" s="38" t="s">
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="43"/>
+    </row>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B2" s="37" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1989,69 +1989,69 @@
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N5" s="35" t="s">
+      <c r="N5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="35"/>
-      <c r="P5" s="35"/>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="27"/>
-      <c r="O6" s="27" t="s">
+      <c r="N6" s="26"/>
+      <c r="O6" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="P6" s="27" t="s">
+      <c r="P6" s="26" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="N7" s="27" t="s">
+      <c r="N7" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="O7" s="27" t="s">
+      <c r="O7" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="P7" s="27">
+      <c r="P7" s="26">
         <v>235</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="N8" s="27" t="s">
+      <c r="N8" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="O8" s="27" t="s">
+      <c r="O8" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="P8" s="27">
+      <c r="P8" s="26">
         <v>235</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="N9" s="27" t="s">
+      <c r="N9" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="O9" s="27"/>
-      <c r="P9" s="27"/>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.45">
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>79</v>
       </c>
@@ -2059,23 +2059,23 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="B11" s="104" t="s">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B11" s="38" t="s">
         <v>78</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
     </row>
   </sheetData>
@@ -2098,89 +2098,89 @@
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="17" max="17" width="10.59765625" customWidth="1"/>
+    <col min="17" max="17" width="10.5546875" customWidth="1"/>
     <col min="19" max="19" width="8" customWidth="1"/>
     <col min="20" max="20" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B1" s="12"/>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="41"/>
-    </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.45">
-      <c r="B3" s="105" t="s">
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="43"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B3" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="44"/>
-    </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.45">
-      <c r="B6" s="39" t="s">
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="49"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B6" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="I6" s="39" t="s">
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="I6" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="40"/>
-      <c r="O6" s="40"/>
-      <c r="Q6" s="39" t="s">
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="42"/>
+      <c r="N6" s="42"/>
+      <c r="O6" s="42"/>
+      <c r="Q6" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="R6" s="40"/>
-      <c r="S6" s="40"/>
-      <c r="T6" s="40"/>
-    </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.45">
-      <c r="B8" s="32" t="s">
+      <c r="R6" s="42"/>
+      <c r="S6" s="42"/>
+      <c r="T6" s="42"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B8" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="56" t="s">
+      <c r="C8" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
       <c r="I8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="Q8" s="55" t="s">
+      <c r="Q8" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="R8" s="55"/>
-      <c r="S8" s="55"/>
-      <c r="T8" s="34">
+      <c r="R8" s="46"/>
+      <c r="S8" s="46"/>
+      <c r="T8" s="33">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.45">
-      <c r="B9" s="35" t="s">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B9" s="34" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="45" t="s">
@@ -2188,20 +2188,20 @@
       </c>
       <c r="D9" s="45"/>
       <c r="E9" s="45"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="I9" s="37"/>
-      <c r="Q9" s="55" t="s">
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="I9" s="36"/>
+      <c r="Q9" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="R9" s="55"/>
-      <c r="S9" s="55"/>
-      <c r="T9" s="34" t="s">
+      <c r="R9" s="46"/>
+      <c r="S9" s="46"/>
+      <c r="T9" s="33" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.45">
-      <c r="B10" s="35" t="s">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B10" s="34" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="45" t="s">
@@ -2209,30 +2209,30 @@
       </c>
       <c r="D10" s="45"/>
       <c r="E10" s="45"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="I10" s="46" t="s">
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="I10" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="47"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="47"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="47"/>
-      <c r="O10" s="48"/>
-      <c r="Q10" s="55" t="s">
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="52"/>
+      <c r="Q10" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="R10" s="55" t="s">
+      <c r="R10" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="S10" s="55"/>
-      <c r="T10" s="34" t="s">
+      <c r="S10" s="46"/>
+      <c r="T10" s="33" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.45">
-      <c r="B11" s="35" t="s">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B11" s="34" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="45" t="s">
@@ -2240,18 +2240,18 @@
       </c>
       <c r="D11" s="45"/>
       <c r="E11" s="45"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
-      <c r="L11" s="50"/>
-      <c r="M11" s="50"/>
-      <c r="N11" s="50"/>
-      <c r="O11" s="51"/>
-    </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.45">
-      <c r="B12" s="35" t="s">
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="54"/>
+      <c r="O11" s="55"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B12" s="34" t="s">
         <v>27</v>
       </c>
       <c r="C12" s="45" t="s">
@@ -2259,18 +2259,18 @@
       </c>
       <c r="D12" s="45"/>
       <c r="E12" s="45"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="50"/>
-      <c r="L12" s="50"/>
-      <c r="M12" s="50"/>
-      <c r="N12" s="50"/>
-      <c r="O12" s="51"/>
-    </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.45">
-      <c r="B13" s="35" t="s">
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="54"/>
+      <c r="L12" s="54"/>
+      <c r="M12" s="54"/>
+      <c r="N12" s="54"/>
+      <c r="O12" s="55"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B13" s="34" t="s">
         <v>28</v>
       </c>
       <c r="C13" s="45" t="s">
@@ -2278,24 +2278,24 @@
       </c>
       <c r="D13" s="45"/>
       <c r="E13" s="45"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="50"/>
-      <c r="K13" s="50"/>
-      <c r="L13" s="50"/>
-      <c r="M13" s="50"/>
-      <c r="N13" s="50"/>
-      <c r="O13" s="51"/>
-      <c r="Q13" s="39" t="s">
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="54"/>
+      <c r="K13" s="54"/>
+      <c r="L13" s="54"/>
+      <c r="M13" s="54"/>
+      <c r="N13" s="54"/>
+      <c r="O13" s="55"/>
+      <c r="Q13" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="R13" s="40"/>
-      <c r="S13" s="40"/>
-      <c r="T13" s="40"/>
-    </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.45">
-      <c r="B14" s="35" t="s">
+      <c r="R13" s="42"/>
+      <c r="S13" s="42"/>
+      <c r="T13" s="42"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B14" s="34" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="45" t="s">
@@ -2303,164 +2303,156 @@
       </c>
       <c r="D14" s="45"/>
       <c r="E14" s="45"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="50"/>
-      <c r="K14" s="50"/>
-      <c r="L14" s="50"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="50"/>
-      <c r="O14" s="51"/>
-    </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.45">
-      <c r="I15" s="49"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="50"/>
-      <c r="L15" s="50"/>
-      <c r="M15" s="50"/>
-      <c r="N15" s="50"/>
-      <c r="O15" s="51"/>
-      <c r="Q15" s="32" t="s">
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="54"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="54"/>
+      <c r="M14" s="54"/>
+      <c r="N14" s="54"/>
+      <c r="O14" s="55"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="I15" s="53"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="54"/>
+      <c r="M15" s="54"/>
+      <c r="N15" s="54"/>
+      <c r="O15" s="55"/>
+      <c r="Q15" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="R15" s="56" t="s">
+      <c r="R15" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="S15" s="56"/>
-      <c r="T15" s="56"/>
-    </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.45">
-      <c r="I16" s="49"/>
-      <c r="J16" s="50"/>
-      <c r="K16" s="50"/>
-      <c r="L16" s="50"/>
-      <c r="M16" s="50"/>
-      <c r="N16" s="50"/>
-      <c r="O16" s="51"/>
-      <c r="Q16" s="35" t="s">
+      <c r="S15" s="59"/>
+      <c r="T15" s="59"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="I16" s="53"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="54"/>
+      <c r="M16" s="54"/>
+      <c r="N16" s="54"/>
+      <c r="O16" s="55"/>
+      <c r="Q16" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="R16" s="42" t="s">
+      <c r="R16" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="S16" s="42"/>
-      <c r="T16" s="42"/>
-    </row>
-    <row r="17" spans="9:20" x14ac:dyDescent="0.45">
-      <c r="I17" s="49"/>
-      <c r="J17" s="50"/>
-      <c r="K17" s="50"/>
-      <c r="L17" s="50"/>
-      <c r="M17" s="50"/>
-      <c r="N17" s="50"/>
-      <c r="O17" s="51"/>
-      <c r="Q17" s="35" t="s">
+      <c r="S16" s="44"/>
+      <c r="T16" s="44"/>
+    </row>
+    <row r="17" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I17" s="53"/>
+      <c r="J17" s="54"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="54"/>
+      <c r="M17" s="54"/>
+      <c r="N17" s="54"/>
+      <c r="O17" s="55"/>
+      <c r="Q17" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="R17" s="42" t="s">
+      <c r="R17" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="S17" s="42"/>
-      <c r="T17" s="42"/>
-    </row>
-    <row r="18" spans="9:20" x14ac:dyDescent="0.45">
-      <c r="I18" s="49"/>
-      <c r="J18" s="50"/>
-      <c r="K18" s="50"/>
-      <c r="L18" s="50"/>
-      <c r="M18" s="50"/>
-      <c r="N18" s="50"/>
-      <c r="O18" s="51"/>
-      <c r="Q18" s="35" t="s">
+      <c r="S17" s="44"/>
+      <c r="T17" s="44"/>
+    </row>
+    <row r="18" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I18" s="53"/>
+      <c r="J18" s="54"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="54"/>
+      <c r="M18" s="54"/>
+      <c r="N18" s="54"/>
+      <c r="O18" s="55"/>
+      <c r="Q18" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="R18" s="42" t="s">
+      <c r="R18" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="S18" s="42"/>
-      <c r="T18" s="42"/>
-    </row>
-    <row r="19" spans="9:20" x14ac:dyDescent="0.45">
-      <c r="I19" s="49"/>
-      <c r="J19" s="50"/>
-      <c r="K19" s="50"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="50"/>
-      <c r="N19" s="50"/>
-      <c r="O19" s="51"/>
-      <c r="Q19" s="35" t="s">
+      <c r="S18" s="44"/>
+      <c r="T18" s="44"/>
+    </row>
+    <row r="19" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I19" s="53"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="54"/>
+      <c r="L19" s="54"/>
+      <c r="M19" s="54"/>
+      <c r="N19" s="54"/>
+      <c r="O19" s="55"/>
+      <c r="Q19" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="R19" s="42" t="s">
+      <c r="R19" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="S19" s="42"/>
-      <c r="T19" s="42"/>
-    </row>
-    <row r="20" spans="9:20" x14ac:dyDescent="0.45">
-      <c r="I20" s="49"/>
-      <c r="J20" s="50"/>
-      <c r="K20" s="50"/>
-      <c r="L20" s="50"/>
-      <c r="M20" s="50"/>
-      <c r="N20" s="50"/>
-      <c r="O20" s="51"/>
-      <c r="Q20" s="35" t="s">
+      <c r="S19" s="44"/>
+      <c r="T19" s="44"/>
+    </row>
+    <row r="20" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I20" s="53"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="54"/>
+      <c r="M20" s="54"/>
+      <c r="N20" s="54"/>
+      <c r="O20" s="55"/>
+      <c r="Q20" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="R20" s="42" t="s">
+      <c r="R20" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="S20" s="42"/>
-      <c r="T20" s="42"/>
-    </row>
-    <row r="21" spans="9:20" x14ac:dyDescent="0.45">
-      <c r="I21" s="49"/>
-      <c r="J21" s="50"/>
-      <c r="K21" s="50"/>
-      <c r="L21" s="50"/>
-      <c r="M21" s="50"/>
-      <c r="N21" s="50"/>
-      <c r="O21" s="51"/>
-    </row>
-    <row r="22" spans="9:20" x14ac:dyDescent="0.45">
-      <c r="I22" s="49"/>
-      <c r="J22" s="50"/>
-      <c r="K22" s="50"/>
-      <c r="L22" s="50"/>
-      <c r="M22" s="50"/>
-      <c r="N22" s="50"/>
-      <c r="O22" s="51"/>
-    </row>
-    <row r="23" spans="9:20" x14ac:dyDescent="0.45">
-      <c r="I23" s="49"/>
-      <c r="J23" s="50"/>
-      <c r="K23" s="50"/>
-      <c r="L23" s="50"/>
-      <c r="M23" s="50"/>
-      <c r="N23" s="50"/>
-      <c r="O23" s="51"/>
-    </row>
-    <row r="24" spans="9:20" x14ac:dyDescent="0.45">
-      <c r="I24" s="52"/>
-      <c r="J24" s="53"/>
-      <c r="K24" s="53"/>
-      <c r="L24" s="53"/>
-      <c r="M24" s="53"/>
-      <c r="N24" s="53"/>
-      <c r="O24" s="54"/>
+      <c r="S20" s="44"/>
+      <c r="T20" s="44"/>
+    </row>
+    <row r="21" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I21" s="53"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="54"/>
+      <c r="M21" s="54"/>
+      <c r="N21" s="54"/>
+      <c r="O21" s="55"/>
+    </row>
+    <row r="22" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I22" s="53"/>
+      <c r="J22" s="54"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="54"/>
+      <c r="M22" s="54"/>
+      <c r="N22" s="54"/>
+      <c r="O22" s="55"/>
+    </row>
+    <row r="23" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I23" s="53"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="54"/>
+      <c r="N23" s="54"/>
+      <c r="O23" s="55"/>
+    </row>
+    <row r="24" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I24" s="56"/>
+      <c r="J24" s="57"/>
+      <c r="K24" s="57"/>
+      <c r="L24" s="57"/>
+      <c r="M24" s="57"/>
+      <c r="N24" s="57"/>
+      <c r="O24" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="Q13:T13"/>
-    <mergeCell ref="C14:E14"/>
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="B3:K3"/>
@@ -2476,6 +2468,14 @@
     <mergeCell ref="Q6:T6"/>
     <mergeCell ref="R17:T17"/>
     <mergeCell ref="R19:T19"/>
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="Q13:T13"/>
+    <mergeCell ref="C14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2490,173 +2490,173 @@
   </sheetPr>
   <dimension ref="B1:W16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="66" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.265625" customWidth="1"/>
-    <col min="3" max="4" width="18.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.1328125" customWidth="1"/>
-    <col min="7" max="7" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1328125" customWidth="1"/>
-    <col min="9" max="9" width="9.265625" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" customWidth="1"/>
+    <col min="3" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.109375" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" customWidth="1"/>
+    <col min="9" max="9" width="9.21875" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="11" max="11" width="7.59765625" customWidth="1"/>
-    <col min="12" max="12" width="10.59765625" customWidth="1"/>
-    <col min="13" max="13" width="13.265625" customWidth="1"/>
-    <col min="14" max="15" width="8.86328125" customWidth="1"/>
+    <col min="11" max="11" width="7.5546875" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" customWidth="1"/>
+    <col min="13" max="13" width="13.21875" customWidth="1"/>
+    <col min="14" max="15" width="8.88671875" customWidth="1"/>
     <col min="19" max="19" width="6" customWidth="1"/>
-    <col min="20" max="20" width="5.53125" customWidth="1"/>
-    <col min="21" max="21" width="6.73046875" customWidth="1"/>
-    <col min="22" max="22" width="7.9296875" customWidth="1"/>
+    <col min="20" max="20" width="5.5546875" customWidth="1"/>
+    <col min="21" max="21" width="6.77734375" customWidth="1"/>
+    <col min="22" max="22" width="7.88671875" customWidth="1"/>
     <col min="23" max="23" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B1" s="12"/>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="41"/>
-    </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.45">
-      <c r="B3" s="105" t="s">
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="43"/>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B3" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="44"/>
-    </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.45">
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="49"/>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B5" s="11"/>
     </row>
-    <row r="6" spans="2:23" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="B6" s="57" t="s">
+    <row r="6" spans="2:23" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="58" t="s">
+      <c r="D6" s="74" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="57" t="s">
+      <c r="E6" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="57"/>
-      <c r="K6" s="57"/>
-      <c r="L6" s="57"/>
-      <c r="M6" s="57"/>
-      <c r="N6" s="57"/>
-      <c r="O6" s="57"/>
-      <c r="P6" s="57"/>
-      <c r="Q6" s="57"/>
-      <c r="R6" s="57"/>
-      <c r="S6" s="57"/>
-      <c r="T6" s="57"/>
-      <c r="U6" s="57"/>
-      <c r="V6" s="57"/>
-      <c r="W6" s="57"/>
-    </row>
-    <row r="7" spans="2:23" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="112" t="s">
+      <c r="F6" s="73"/>
+      <c r="G6" s="73"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="73"/>
+      <c r="J6" s="73"/>
+      <c r="K6" s="73"/>
+      <c r="L6" s="73"/>
+      <c r="M6" s="73"/>
+      <c r="N6" s="73"/>
+      <c r="O6" s="73"/>
+      <c r="P6" s="73"/>
+      <c r="Q6" s="73"/>
+      <c r="R6" s="73"/>
+      <c r="S6" s="73"/>
+      <c r="T6" s="73"/>
+      <c r="U6" s="73"/>
+      <c r="V6" s="73"/>
+      <c r="W6" s="73"/>
+    </row>
+    <row r="7" spans="2:23" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="64" t="s">
+      <c r="F7" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="64"/>
-      <c r="H7" s="64"/>
-      <c r="I7" s="64"/>
-      <c r="J7" s="64"/>
-      <c r="K7" s="64"/>
-      <c r="L7" s="64"/>
-      <c r="M7" s="64"/>
-      <c r="N7" s="61" t="s">
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="67"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="67"/>
+      <c r="N7" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="O7" s="61"/>
-      <c r="P7" s="61"/>
-      <c r="Q7" s="61"/>
-      <c r="R7" s="61"/>
-      <c r="S7" s="60" t="s">
+      <c r="O7" s="68"/>
+      <c r="P7" s="68"/>
+      <c r="Q7" s="68"/>
+      <c r="R7" s="68"/>
+      <c r="S7" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="T7" s="60"/>
-      <c r="U7" s="60"/>
-      <c r="V7" s="60"/>
-      <c r="W7" s="60"/>
-    </row>
-    <row r="8" spans="2:23" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="57"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="113"/>
-      <c r="F8" s="110" t="s">
+      <c r="T7" s="76"/>
+      <c r="U7" s="76"/>
+      <c r="V7" s="76"/>
+      <c r="W7" s="76"/>
+    </row>
+    <row r="8" spans="2:23" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="73"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="G8" s="111"/>
-      <c r="H8" s="110" t="s">
+      <c r="G8" s="63"/>
+      <c r="H8" s="62" t="s">
         <v>94</v>
       </c>
-      <c r="I8" s="111"/>
-      <c r="J8" s="110" t="s">
+      <c r="I8" s="63"/>
+      <c r="J8" s="62" t="s">
         <v>96</v>
       </c>
-      <c r="K8" s="111"/>
-      <c r="L8" s="110" t="s">
+      <c r="K8" s="63"/>
+      <c r="L8" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="M8" s="111"/>
-      <c r="N8" s="106" t="s">
+      <c r="M8" s="63"/>
+      <c r="N8" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="O8" s="106" t="s">
+      <c r="O8" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="P8" s="106" t="s">
+      <c r="P8" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="Q8" s="106" t="s">
+      <c r="Q8" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="R8" s="106" t="s">
+      <c r="R8" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="S8" s="108">
+      <c r="S8" s="69">
         <v>0</v>
       </c>
-      <c r="T8" s="108">
+      <c r="T8" s="69">
         <v>1</v>
       </c>
-      <c r="U8" s="108">
+      <c r="U8" s="69">
         <v>2</v>
       </c>
-      <c r="V8" s="108" t="s">
+      <c r="V8" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="W8" s="108" t="s">
+      <c r="W8" s="69" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="2:23" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="B9" s="57"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="114"/>
+    <row r="9" spans="2:23" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="73"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="66"/>
       <c r="F9" s="13" t="s">
         <v>45</v>
       </c>
@@ -2681,18 +2681,18 @@
       <c r="M9" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="N9" s="107"/>
-      <c r="O9" s="107"/>
-      <c r="P9" s="107"/>
-      <c r="Q9" s="107"/>
-      <c r="R9" s="107"/>
-      <c r="S9" s="109"/>
-      <c r="T9" s="109"/>
-      <c r="U9" s="109"/>
-      <c r="V9" s="109"/>
-      <c r="W9" s="109"/>
-    </row>
-    <row r="10" spans="2:23" ht="15.75" x14ac:dyDescent="0.45">
+      <c r="N9" s="72"/>
+      <c r="O9" s="72"/>
+      <c r="P9" s="72"/>
+      <c r="Q9" s="72"/>
+      <c r="R9" s="72"/>
+      <c r="S9" s="70"/>
+      <c r="T9" s="70"/>
+      <c r="U9" s="70"/>
+      <c r="V9" s="70"/>
+      <c r="W9" s="70"/>
+    </row>
+    <row r="10" spans="2:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="14" t="s">
         <v>47</v>
       </c>
@@ -2744,7 +2744,7 @@
       <c r="V10" s="19"/>
       <c r="W10" s="19"/>
     </row>
-    <row r="11" spans="2:23" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="14" t="s">
         <v>48</v>
       </c>
@@ -2796,14 +2796,14 @@
       <c r="V11" s="19"/>
       <c r="W11" s="19"/>
     </row>
-    <row r="12" spans="2:23" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:23" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B12" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="115" t="s">
+      <c r="C12" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="D12" s="116" t="s">
+      <c r="D12" s="40" t="s">
         <v>99</v>
       </c>
       <c r="E12" s="16" t="s">
@@ -2848,7 +2848,7 @@
       <c r="V12" s="19"/>
       <c r="W12" s="19"/>
     </row>
-    <row r="13" spans="2:23" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:23" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B13" s="14" t="s">
         <v>91</v>
       </c>
@@ -2900,7 +2900,7 @@
       <c r="V13" s="19"/>
       <c r="W13" s="19"/>
     </row>
-    <row r="14" spans="2:23" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:23" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B14" s="14" t="s">
         <v>92</v>
       </c>
@@ -2952,23 +2952,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="2:23" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:M7"/>
-    <mergeCell ref="N7:R7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="S8:S9"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B6:B9"/>
@@ -2983,6 +2971,18 @@
     <mergeCell ref="V8:V9"/>
     <mergeCell ref="R8:R9"/>
     <mergeCell ref="S7:W7"/>
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:M7"/>
+    <mergeCell ref="N7:R7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2996,76 +2996,76 @@
   </sheetPr>
   <dimension ref="B1:N16"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" zoomScale="128" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14:M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="7.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.1328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.1328125" customWidth="1"/>
-    <col min="13" max="13" width="16.1328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.265625" customWidth="1"/>
+    <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" customWidth="1"/>
+    <col min="13" max="13" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B1" s="12"/>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="41"/>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B3" s="67" t="s">
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="43"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B3" s="101" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="67"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B4" s="68" t="s">
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="101"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B4" s="102" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="88" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="79" t="s">
+      <c r="D4" s="112" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="70" t="s">
+      <c r="E4" s="104" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="70" t="s">
+      <c r="F4" s="110"/>
+      <c r="G4" s="110"/>
+      <c r="H4" s="110"/>
+      <c r="I4" s="110"/>
+      <c r="J4" s="105"/>
+      <c r="K4" s="104" t="s">
         <v>54</v>
       </c>
-      <c r="L4" s="71"/>
-    </row>
-    <row r="5" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="69"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="80"/>
+      <c r="L4" s="105"/>
+    </row>
+    <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="103"/>
+      <c r="C5" s="111"/>
+      <c r="D5" s="113"/>
       <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
@@ -3078,10 +3078,10 @@
       <c r="H5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="72" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="73"/>
+      <c r="I5" s="106" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="107"/>
       <c r="K5" s="2" t="s">
         <v>55</v>
       </c>
@@ -3089,11 +3089,11 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B6" s="21">
         <v>9</v>
       </c>
-      <c r="C6" s="74" t="s">
+      <c r="C6" s="108" t="s">
         <v>57</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -3111,10 +3111,10 @@
       <c r="H6" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="81" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="82"/>
+      <c r="I6" s="114" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="115"/>
       <c r="K6" s="22" t="s">
         <v>19</v>
       </c>
@@ -3122,11 +3122,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="21">
         <v>10</v>
       </c>
-      <c r="C7" s="74"/>
+      <c r="C7" s="108"/>
       <c r="D7" s="4" t="s">
         <v>58</v>
       </c>
@@ -3142,10 +3142,10 @@
       <c r="H7" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="70" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="71"/>
+      <c r="I7" s="104" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="105"/>
       <c r="K7" s="21" t="s">
         <v>19</v>
       </c>
@@ -3153,11 +3153,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="21">
         <v>11</v>
       </c>
-      <c r="C8" s="74"/>
+      <c r="C8" s="108"/>
       <c r="D8" s="10" t="s">
         <v>19</v>
       </c>
@@ -3173,10 +3173,10 @@
       <c r="H8" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="70" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="71"/>
+      <c r="I8" s="104" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="105"/>
       <c r="K8" s="21" t="s">
         <v>19</v>
       </c>
@@ -3184,11 +3184,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="21">
         <v>12</v>
       </c>
-      <c r="C9" s="74"/>
+      <c r="C9" s="108"/>
       <c r="D9" s="10" t="s">
         <v>19</v>
       </c>
@@ -3204,10 +3204,10 @@
       <c r="H9" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="70" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" s="71"/>
+      <c r="I9" s="104" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="105"/>
       <c r="K9" s="21" t="s">
         <v>19</v>
       </c>
@@ -3215,11 +3215,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="2">
         <v>13</v>
       </c>
-      <c r="C10" s="75"/>
+      <c r="C10" s="109"/>
       <c r="D10" s="9" t="s">
         <v>19</v>
       </c>
@@ -3235,10 +3235,10 @@
       <c r="H10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="72" t="s">
-        <v>19</v>
-      </c>
-      <c r="J10" s="73"/>
+      <c r="I10" s="106" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="107"/>
       <c r="K10" s="2" t="s">
         <v>19</v>
       </c>
@@ -3246,7 +3246,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:14" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -3259,49 +3259,49 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
         <v>59</v>
       </c>
       <c r="K12" s="23"/>
     </row>
-    <row r="13" spans="2:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B13" s="83" t="s">
+    <row r="13" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="93" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="84"/>
-      <c r="D13" s="84"/>
-      <c r="E13" s="84"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="94"/>
       <c r="F13" s="85" t="s">
         <v>61</v>
       </c>
       <c r="G13" s="86"/>
-      <c r="H13" s="83" t="s">
+      <c r="H13" s="93" t="s">
         <v>62</v>
       </c>
-      <c r="I13" s="84"/>
-      <c r="J13" s="84"/>
-      <c r="K13" s="84"/>
-      <c r="L13" s="100"/>
-      <c r="M13" s="65" t="s">
+      <c r="I13" s="94"/>
+      <c r="J13" s="94"/>
+      <c r="K13" s="94"/>
+      <c r="L13" s="95"/>
+      <c r="M13" s="99" t="s">
         <v>63</v>
       </c>
-      <c r="N13" s="66"/>
-    </row>
-    <row r="14" spans="2:14" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="95" t="s">
+      <c r="N13" s="100"/>
+    </row>
+    <row r="14" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="77" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="91" t="s">
+      <c r="C14" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="91" t="s">
+      <c r="D14" s="79" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="97" t="s">
+      <c r="E14" s="81" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="88" t="s">
+      <c r="F14" s="83" t="s">
         <v>68</v>
       </c>
       <c r="G14" s="87" t="s">
@@ -3310,42 +3310,42 @@
       <c r="H14" s="89" t="s">
         <v>70</v>
       </c>
-      <c r="I14" s="91" t="s">
+      <c r="I14" s="79" t="s">
         <v>64</v>
       </c>
-      <c r="J14" s="91" t="s">
+      <c r="J14" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="K14" s="93" t="s">
+      <c r="K14" s="91" t="s">
         <v>71</v>
       </c>
-      <c r="L14" s="101" t="s">
+      <c r="L14" s="96" t="s">
         <v>72</v>
       </c>
-      <c r="M14" s="103" t="s">
+      <c r="M14" s="98" t="s">
         <v>73</v>
       </c>
-      <c r="N14" s="77" t="s">
+      <c r="N14" s="88" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B15" s="96"/>
-      <c r="C15" s="92"/>
-      <c r="D15" s="92"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="99"/>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B15" s="78"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="82"/>
+      <c r="F15" s="84"/>
       <c r="G15" s="87"/>
       <c r="H15" s="90"/>
-      <c r="I15" s="92"/>
-      <c r="J15" s="92"/>
-      <c r="K15" s="94"/>
-      <c r="L15" s="102"/>
-      <c r="M15" s="95"/>
-      <c r="N15" s="88"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B16" s="27">
+      <c r="I15" s="80"/>
+      <c r="J15" s="80"/>
+      <c r="K15" s="92"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="77"/>
+      <c r="N15" s="83"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B16" s="26">
         <f>SUM(C16:D16)</f>
         <v>5</v>
       </c>
@@ -3355,8 +3355,10 @@
       <c r="D16" s="24">
         <v>0</v>
       </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="26">
+      <c r="E16" s="116">
+        <v>0.67</v>
+      </c>
+      <c r="F16" s="25">
         <v>0</v>
       </c>
       <c r="G16" s="8" t="s">
@@ -3365,43 +3367,28 @@
       <c r="H16" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="I16" s="27">
+      <c r="I16" s="26">
         <f>SUM(J16:K16)</f>
         <v>0</v>
       </c>
       <c r="J16" s="24">
         <v>0</v>
       </c>
-      <c r="K16" s="28">
+      <c r="K16" s="27">
         <v>0</v>
       </c>
-      <c r="L16" s="29"/>
+      <c r="L16" s="28"/>
       <c r="M16" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="N16" s="30">
+      <c r="N16" s="29">
         <f>C16</f>
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="B13:E13"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:L3"/>
     <mergeCell ref="B4:B5"/>
@@ -3416,7 +3403,22 @@
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="I8:J8"/>
-    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3424,21 +3426,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010058284A30843C9F43BD758DDD8294D484" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2e00392fbb7f49de63e89755c965b762">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fed1744a-f275-4023-9290-77fd546fd730" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="37d4e1d93698397f16b7bbb6f83014a7" ns2:_="">
     <xsd:import namespace="fed1744a-f275-4023-9290-77fd546fd730"/>
@@ -3606,24 +3593,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5426D20B-58AE-4BE9-8733-DFB2BC19D8C6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6597AB9C-DC10-4824-8900-518D3B18165A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{845501DA-8B32-4FE5-8083-FBCE9B17F25B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3639,4 +3624,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6597AB9C-DC10-4824-8900-518D3B18165A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5426D20B-58AE-4BE9-8733-DFB2BC19D8C6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
lab 04 mockito + junit + test link
</commit_message>
<xml_diff>
--- a/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
+++ b/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213A449E-79E1-4BAD-8603-2812D3CDD800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B56921-83F6-489A-8038-1F101BB02D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -372,9 +372,6 @@
     <t>F02.getTotalAmount(PaymentType type)</t>
   </si>
   <si>
-    <t>11 - 10 + 2 = 3</t>
-  </si>
-  <si>
     <t>4+1 = 5</t>
   </si>
   <si>
@@ -481,6 +478,9 @@
   </si>
   <si>
     <t>200.0</t>
+  </si>
+  <si>
+    <t>13 - 10 + 2 = 5</t>
   </si>
 </sst>
 </file>
@@ -1216,69 +1216,87 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1296,23 +1314,38 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1353,9 +1386,6 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1366,36 +1396,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1417,56 +1417,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>21646</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>89298</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>124475</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>129886</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{675E7CC8-1A8A-753A-C468-AF666157BDE7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5168394" y="1160861"/>
-          <a:ext cx="4535200" cy="4148244"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1494,7 +1444,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1503,6 +1453,50 @@
         <a:xfrm>
           <a:off x="476250" y="1272886"/>
           <a:ext cx="4124967" cy="2000529"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>337706</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>77931</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>207819</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>130011</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28B4F698-9B78-BB45-012C-C2BBA67E464A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4658592" y="1714499"/>
+          <a:ext cx="4719204" cy="2597853"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1944,8 +1938,8 @@
   </sheetPr>
   <dimension ref="B1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="88" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1968,18 +1962,18 @@
       <c r="I1" s="42"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="48"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="46"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B6" s="40" t="s">
@@ -2020,11 +2014,11 @@
       <c r="I8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="Q8" s="44" t="s">
+      <c r="Q8" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="R8" s="44"/>
-      <c r="S8" s="44"/>
+      <c r="R8" s="57"/>
+      <c r="S8" s="57"/>
       <c r="T8" s="30">
         <v>5</v>
       </c>
@@ -2033,110 +2027,110 @@
       <c r="B9" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
       <c r="F9" s="32"/>
       <c r="G9" s="32"/>
       <c r="I9" s="33"/>
-      <c r="Q9" s="44" t="s">
+      <c r="Q9" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="R9" s="44"/>
-      <c r="S9" s="44"/>
+      <c r="R9" s="57"/>
+      <c r="S9" s="57"/>
       <c r="T9" s="30" t="s">
-        <v>76</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B10" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
       <c r="F10" s="32"/>
       <c r="G10" s="32"/>
-      <c r="I10" s="49" t="s">
+      <c r="I10" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="50"/>
-      <c r="K10" s="50"/>
-      <c r="L10" s="50"/>
-      <c r="M10" s="50"/>
-      <c r="N10" s="50"/>
-      <c r="O10" s="51"/>
-      <c r="Q10" s="44" t="s">
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="49"/>
+      <c r="N10" s="49"/>
+      <c r="O10" s="50"/>
+      <c r="Q10" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="R10" s="44" t="s">
+      <c r="R10" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="S10" s="44"/>
+      <c r="S10" s="57"/>
       <c r="T10" s="30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B11" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
       <c r="F11" s="32"/>
       <c r="G11" s="32"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="53"/>
-      <c r="N11" s="53"/>
-      <c r="O11" s="54"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="52"/>
+      <c r="O11" s="53"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B12" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
       <c r="F12" s="32"/>
       <c r="G12" s="32"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="53"/>
-      <c r="N12" s="53"/>
-      <c r="O12" s="54"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="52"/>
+      <c r="O12" s="53"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B13" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="43" t="s">
+      <c r="C13" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
       <c r="F13" s="32"/>
       <c r="G13" s="32"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="53"/>
-      <c r="L13" s="53"/>
-      <c r="M13" s="53"/>
-      <c r="N13" s="53"/>
-      <c r="O13" s="54"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="52"/>
+      <c r="L13" s="52"/>
+      <c r="M13" s="52"/>
+      <c r="N13" s="52"/>
+      <c r="O13" s="53"/>
       <c r="Q13" s="40" t="s">
         <v>29</v>
       </c>
@@ -2148,29 +2142,29 @@
       <c r="B14" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
       <c r="F14" s="32"/>
       <c r="G14" s="32"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="53"/>
-      <c r="L14" s="53"/>
-      <c r="M14" s="53"/>
-      <c r="N14" s="53"/>
-      <c r="O14" s="54"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="52"/>
+      <c r="N14" s="52"/>
+      <c r="O14" s="53"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="I15" s="52"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="53"/>
-      <c r="L15" s="53"/>
-      <c r="M15" s="53"/>
-      <c r="N15" s="53"/>
-      <c r="O15" s="54"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="52"/>
+      <c r="L15" s="52"/>
+      <c r="M15" s="52"/>
+      <c r="N15" s="52"/>
+      <c r="O15" s="53"/>
       <c r="Q15" s="28" t="s">
         <v>30</v>
       </c>
@@ -2181,128 +2175,135 @@
       <c r="T15" s="58"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="I16" s="52"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="53"/>
-      <c r="L16" s="53"/>
-      <c r="M16" s="53"/>
-      <c r="N16" s="53"/>
-      <c r="O16" s="54"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="52"/>
+      <c r="N16" s="52"/>
+      <c r="O16" s="53"/>
       <c r="Q16" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="R16" s="45" t="s">
-        <v>78</v>
-      </c>
-      <c r="S16" s="45"/>
-      <c r="T16" s="45"/>
+      <c r="R16" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="S16" s="43"/>
+      <c r="T16" s="43"/>
     </row>
     <row r="17" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I17" s="52"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="53"/>
-      <c r="L17" s="53"/>
-      <c r="M17" s="53"/>
-      <c r="N17" s="53"/>
-      <c r="O17" s="54"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="52"/>
+      <c r="N17" s="52"/>
+      <c r="O17" s="53"/>
       <c r="Q17" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="R17" s="45" t="s">
-        <v>79</v>
-      </c>
-      <c r="S17" s="45"/>
-      <c r="T17" s="45"/>
+      <c r="R17" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="S17" s="43"/>
+      <c r="T17" s="43"/>
     </row>
     <row r="18" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I18" s="52"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="53"/>
-      <c r="L18" s="53"/>
-      <c r="M18" s="53"/>
-      <c r="N18" s="53"/>
-      <c r="O18" s="54"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="52"/>
+      <c r="L18" s="52"/>
+      <c r="M18" s="52"/>
+      <c r="N18" s="52"/>
+      <c r="O18" s="53"/>
       <c r="Q18" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="R18" s="45" t="s">
+      <c r="R18" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="S18" s="43"/>
+      <c r="T18" s="43"/>
+    </row>
+    <row r="19" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I19" s="51"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="52"/>
+      <c r="N19" s="52"/>
+      <c r="O19" s="53"/>
+      <c r="Q19" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="S18" s="45"/>
-      <c r="T18" s="45"/>
-    </row>
-    <row r="19" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I19" s="52"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="53"/>
-      <c r="L19" s="53"/>
-      <c r="M19" s="53"/>
-      <c r="N19" s="53"/>
-      <c r="O19" s="54"/>
-      <c r="Q19" s="31" t="s">
+      <c r="R19" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="R19" s="45" t="s">
+      <c r="S19" s="43"/>
+      <c r="T19" s="43"/>
+    </row>
+    <row r="20" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I20" s="51"/>
+      <c r="J20" s="52"/>
+      <c r="K20" s="52"/>
+      <c r="L20" s="52"/>
+      <c r="M20" s="52"/>
+      <c r="N20" s="52"/>
+      <c r="O20" s="53"/>
+      <c r="Q20" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="S19" s="45"/>
-      <c r="T19" s="45"/>
-    </row>
-    <row r="20" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I20" s="52"/>
-      <c r="J20" s="53"/>
-      <c r="K20" s="53"/>
-      <c r="L20" s="53"/>
-      <c r="M20" s="53"/>
-      <c r="N20" s="53"/>
-      <c r="O20" s="54"/>
-      <c r="Q20" s="31" t="s">
+      <c r="R20" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="R20" s="45" t="s">
-        <v>84</v>
-      </c>
-      <c r="S20" s="45"/>
-      <c r="T20" s="45"/>
+      <c r="S20" s="43"/>
+      <c r="T20" s="43"/>
     </row>
     <row r="21" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I21" s="52"/>
-      <c r="J21" s="53"/>
-      <c r="K21" s="53"/>
-      <c r="L21" s="53"/>
-      <c r="M21" s="53"/>
-      <c r="N21" s="53"/>
-      <c r="O21" s="54"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="52"/>
+      <c r="L21" s="52"/>
+      <c r="M21" s="52"/>
+      <c r="N21" s="52"/>
+      <c r="O21" s="53"/>
     </row>
     <row r="22" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I22" s="52"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="53"/>
-      <c r="L22" s="53"/>
-      <c r="M22" s="53"/>
-      <c r="N22" s="53"/>
-      <c r="O22" s="54"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="52"/>
+      <c r="K22" s="52"/>
+      <c r="L22" s="52"/>
+      <c r="M22" s="52"/>
+      <c r="N22" s="52"/>
+      <c r="O22" s="53"/>
     </row>
     <row r="23" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I23" s="52"/>
-      <c r="J23" s="53"/>
-      <c r="K23" s="53"/>
-      <c r="L23" s="53"/>
-      <c r="M23" s="53"/>
-      <c r="N23" s="53"/>
-      <c r="O23" s="54"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="52"/>
+      <c r="N23" s="52"/>
+      <c r="O23" s="53"/>
     </row>
     <row r="24" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I24" s="55"/>
-      <c r="J24" s="56"/>
-      <c r="K24" s="56"/>
-      <c r="L24" s="56"/>
-      <c r="M24" s="56"/>
-      <c r="N24" s="56"/>
-      <c r="O24" s="57"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="55"/>
+      <c r="K24" s="55"/>
+      <c r="L24" s="55"/>
+      <c r="M24" s="55"/>
+      <c r="N24" s="55"/>
+      <c r="O24" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="Q13:T13"/>
+    <mergeCell ref="C14:E14"/>
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="B3:K3"/>
@@ -2319,13 +2320,6 @@
     <mergeCell ref="R17:T17"/>
     <mergeCell ref="R19:T19"/>
     <mergeCell ref="R18:T18"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="Q13:T13"/>
-    <mergeCell ref="C14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2375,138 +2369,138 @@
       <c r="G1" s="42"/>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="48"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="46"/>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B5" s="9"/>
     </row>
     <row r="6" spans="2:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="70" t="s">
+      <c r="C6" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="71" t="s">
+      <c r="D6" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="70" t="s">
+      <c r="E6" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="70"/>
-      <c r="L6" s="70"/>
-      <c r="M6" s="70"/>
-      <c r="N6" s="70"/>
-      <c r="O6" s="70"/>
-      <c r="P6" s="70"/>
-      <c r="Q6" s="70"/>
-      <c r="R6" s="70"/>
-      <c r="S6" s="70"/>
-      <c r="T6" s="70"/>
-      <c r="U6" s="70"/>
-      <c r="V6" s="70"/>
-      <c r="W6" s="70"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="59"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="59"/>
+      <c r="P6" s="59"/>
+      <c r="Q6" s="59"/>
+      <c r="R6" s="59"/>
+      <c r="S6" s="59"/>
+      <c r="T6" s="59"/>
+      <c r="U6" s="59"/>
+      <c r="V6" s="59"/>
+      <c r="W6" s="59"/>
     </row>
     <row r="7" spans="2:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="65" t="s">
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="68" t="s">
+      <c r="F7" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="68"/>
-      <c r="H7" s="68"/>
-      <c r="I7" s="68"/>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
-      <c r="L7" s="68"/>
-      <c r="M7" s="68"/>
-      <c r="N7" s="69" t="s">
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="74"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="O7" s="69"/>
-      <c r="P7" s="69"/>
-      <c r="Q7" s="69"/>
-      <c r="R7" s="69"/>
-      <c r="S7" s="75" t="s">
+      <c r="O7" s="75"/>
+      <c r="P7" s="75"/>
+      <c r="Q7" s="75"/>
+      <c r="R7" s="75"/>
+      <c r="S7" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="T7" s="75"/>
-      <c r="U7" s="75"/>
-      <c r="V7" s="75"/>
-      <c r="W7" s="75"/>
+      <c r="T7" s="70"/>
+      <c r="U7" s="70"/>
+      <c r="V7" s="70"/>
+      <c r="W7" s="70"/>
     </row>
     <row r="8" spans="2:23" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="70"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="63" t="s">
+      <c r="B8" s="59"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="66" t="s">
+        <v>87</v>
+      </c>
+      <c r="G8" s="67"/>
+      <c r="H8" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="G8" s="64"/>
-      <c r="H8" s="63" t="s">
-        <v>89</v>
-      </c>
-      <c r="I8" s="64"/>
-      <c r="J8" s="63" t="s">
+      <c r="I8" s="67"/>
+      <c r="J8" s="66" t="s">
+        <v>90</v>
+      </c>
+      <c r="K8" s="67"/>
+      <c r="L8" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="K8" s="64"/>
-      <c r="L8" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="M8" s="64"/>
-      <c r="N8" s="59" t="s">
+      <c r="M8" s="67"/>
+      <c r="N8" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="O8" s="59" t="s">
+      <c r="O8" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="P8" s="59" t="s">
+      <c r="P8" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="Q8" s="59" t="s">
-        <v>81</v>
-      </c>
-      <c r="R8" s="59" t="s">
-        <v>83</v>
-      </c>
-      <c r="S8" s="73">
+      <c r="Q8" s="68" t="s">
+        <v>80</v>
+      </c>
+      <c r="R8" s="68" t="s">
+        <v>82</v>
+      </c>
+      <c r="S8" s="62">
         <v>0</v>
       </c>
-      <c r="T8" s="73">
+      <c r="T8" s="62">
         <v>1</v>
       </c>
-      <c r="U8" s="73">
+      <c r="U8" s="62">
         <v>2</v>
       </c>
-      <c r="V8" s="73" t="s">
+      <c r="V8" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="W8" s="73" t="s">
+      <c r="W8" s="62" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" spans="2:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="70"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="67"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="73"/>
       <c r="F9" s="11" t="s">
         <v>45</v>
       </c>
@@ -2531,63 +2525,63 @@
       <c r="M9" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="N9" s="60"/>
-      <c r="O9" s="60"/>
-      <c r="P9" s="60"/>
-      <c r="Q9" s="60"/>
-      <c r="R9" s="60"/>
-      <c r="S9" s="74"/>
-      <c r="T9" s="74"/>
-      <c r="U9" s="74"/>
-      <c r="V9" s="74"/>
-      <c r="W9" s="74"/>
+      <c r="N9" s="69"/>
+      <c r="O9" s="69"/>
+      <c r="P9" s="69"/>
+      <c r="Q9" s="69"/>
+      <c r="R9" s="69"/>
+      <c r="S9" s="63"/>
+      <c r="T9" s="63"/>
+      <c r="U9" s="63"/>
+      <c r="V9" s="63"/>
+      <c r="W9" s="63"/>
     </row>
     <row r="10" spans="2:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="12" t="s">
         <v>47</v>
       </c>
       <c r="C10" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>94</v>
-      </c>
       <c r="E10" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>45</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K10" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L10" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N10" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O10" s="16"/>
       <c r="P10" s="16"/>
       <c r="Q10" s="16"/>
       <c r="R10" s="16"/>
       <c r="S10" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="T10" s="17"/>
       <c r="U10" s="17"/>
@@ -2599,16 +2593,16 @@
         <v>48</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G11" s="15" t="s">
         <v>46</v>
@@ -2617,29 +2611,29 @@
         <v>45</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K11" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L11" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M11" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N11" s="16"/>
       <c r="O11" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P11" s="16"/>
       <c r="Q11" s="16"/>
       <c r="R11" s="16"/>
       <c r="S11" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="T11" s="17"/>
       <c r="U11" s="17"/>
@@ -2648,25 +2642,25 @@
     </row>
     <row r="12" spans="2:23" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B12" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G12" s="15" t="s">
         <v>46</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I12" s="15" t="s">
         <v>46</v>
@@ -2675,10 +2669,10 @@
         <v>45</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M12" s="15" t="s">
         <v>46</v>
@@ -2686,13 +2680,13 @@
       <c r="N12" s="16"/>
       <c r="O12" s="16"/>
       <c r="P12" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
       <c r="S12" s="17"/>
       <c r="T12" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U12" s="17"/>
       <c r="V12" s="17"/>
@@ -2700,31 +2694,31 @@
     </row>
     <row r="13" spans="2:23" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B13" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>46</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I13" s="15" t="s">
         <v>46</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K13" s="15" t="s">
         <v>46</v>
@@ -2733,44 +2727,44 @@
         <v>45</v>
       </c>
       <c r="M13" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N13" s="16"/>
       <c r="O13" s="16"/>
       <c r="P13" s="16"/>
       <c r="Q13" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="R13" s="16"/>
       <c r="S13" s="17"/>
       <c r="T13" s="17"/>
       <c r="U13" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="V13" s="17"/>
       <c r="W13" s="17"/>
     </row>
     <row r="14" spans="2:23" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B14" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C14" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>99</v>
-      </c>
       <c r="E14" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G14" s="15" t="s">
         <v>46</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I14" s="15" t="s">
         <v>46</v>
@@ -2779,7 +2773,7 @@
         <v>45</v>
       </c>
       <c r="K14" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L14" s="15" t="s">
         <v>45</v>
@@ -2792,14 +2786,14 @@
       <c r="P14" s="16"/>
       <c r="Q14" s="16"/>
       <c r="R14" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S14" s="17"/>
       <c r="T14" s="17"/>
       <c r="U14" s="17"/>
       <c r="V14" s="17"/>
       <c r="W14" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="2:23" ht="15.6" x14ac:dyDescent="0.3">
@@ -2807,6 +2801,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:M7"/>
+    <mergeCell ref="N7:R7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B6:B9"/>
@@ -2823,16 +2827,6 @@
     <mergeCell ref="S7:W7"/>
     <mergeCell ref="S8:S9"/>
     <mergeCell ref="N8:N9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:M7"/>
-    <mergeCell ref="N7:R7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2869,39 +2863,39 @@
       <c r="E1" s="41"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="94" t="s">
+      <c r="B3" s="76" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="77" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="89" t="s">
+      <c r="C4" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="102" t="s">
+      <c r="D4" s="85" t="s">
         <v>52</v>
       </c>
       <c r="E4" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="97" t="s">
+      <c r="F4" s="79" t="s">
         <v>54</v>
       </c>
-      <c r="G4" s="98"/>
+      <c r="G4" s="80"/>
     </row>
     <row r="5" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="96"/>
-      <c r="C5" s="101"/>
-      <c r="D5" s="103"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="86"/>
       <c r="E5" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>55</v>
@@ -2914,92 +2908,92 @@
       <c r="B6" s="19">
         <v>9</v>
       </c>
-      <c r="C6" s="99" t="s">
+      <c r="C6" s="81" t="s">
         <v>57</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>47</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="19">
         <v>10</v>
       </c>
-      <c r="C7" s="99"/>
+      <c r="C7" s="81"/>
       <c r="D7" s="4" t="s">
         <v>58</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="19">
         <v>11</v>
       </c>
-      <c r="C8" s="99"/>
+      <c r="C8" s="81"/>
       <c r="D8" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="19">
         <v>12</v>
       </c>
-      <c r="C9" s="99"/>
+      <c r="C9" s="81"/>
       <c r="D9" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="2">
         <v>13</v>
       </c>
-      <c r="C10" s="100"/>
+      <c r="C10" s="82"/>
       <c r="D10" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="F10" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -3017,54 +3011,54 @@
       <c r="F12" s="21"/>
     </row>
     <row r="13" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="93" t="s">
+      <c r="B13" s="103" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="76"/>
-      <c r="D13" s="76"/>
-      <c r="E13" s="76"/>
-      <c r="F13" s="76"/>
-      <c r="G13" s="77"/>
-      <c r="H13" s="82" t="s">
+      <c r="C13" s="87"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="87"/>
+      <c r="F13" s="87"/>
+      <c r="G13" s="88"/>
+      <c r="H13" s="93" t="s">
         <v>61</v>
       </c>
-      <c r="I13" s="83"/>
+      <c r="I13" s="94"/>
     </row>
     <row r="14" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="81" t="s">
+      <c r="B14" s="92" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="85" t="s">
+      <c r="C14" s="96" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="85" t="s">
+      <c r="D14" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="87" t="s">
+      <c r="E14" s="98" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="91" t="s">
+      <c r="F14" s="101" t="s">
         <v>66</v>
       </c>
-      <c r="G14" s="78" t="s">
+      <c r="G14" s="89" t="s">
         <v>67</v>
       </c>
-      <c r="H14" s="80" t="s">
+      <c r="H14" s="91" t="s">
         <v>68</v>
       </c>
-      <c r="I14" s="89" t="s">
+      <c r="I14" s="83" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="84"/>
-      <c r="C15" s="86"/>
-      <c r="D15" s="86"/>
-      <c r="E15" s="88"/>
-      <c r="F15" s="92"/>
-      <c r="G15" s="79"/>
-      <c r="H15" s="81"/>
-      <c r="I15" s="90"/>
+      <c r="B15" s="95"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="99"/>
+      <c r="F15" s="102"/>
+      <c r="G15" s="90"/>
+      <c r="H15" s="92"/>
+      <c r="I15" s="100"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="23">
@@ -3094,13 +3088,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="H14:H15"/>
@@ -3112,6 +3099,13 @@
     <mergeCell ref="I14:I15"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="B13:E13"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3119,6 +3113,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010058284A30843C9F43BD758DDD8294D484" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2e00392fbb7f49de63e89755c965b762">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fed1744a-f275-4023-9290-77fd546fd730" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="37d4e1d93698397f16b7bbb6f83014a7" ns2:_="">
     <xsd:import namespace="fed1744a-f275-4023-9290-77fd546fd730"/>
@@ -3286,22 +3295,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5426D20B-58AE-4BE9-8733-DFB2BC19D8C6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6597AB9C-DC10-4824-8900-518D3B18165A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{845501DA-8B32-4FE5-8083-FBCE9B17F25B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3317,21 +3328,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6597AB9C-DC10-4824-8900-518D3B18165A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5426D20B-58AE-4BE9-8733-DFB2BC19D8C6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>